<commit_message>
Tweaked AI test files to run without requiring app instantiation, added commentary to flagged data testing notebook
</commit_message>
<xml_diff>
--- a/app/AI Testing Files/Output_Files/Testing Set.xlsx
+++ b/app/AI Testing Files/Output_Files/Testing Set.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H66"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,20 +456,25 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>credit points</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>position</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>flag</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>AI_Flag</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Suggested Rewrite</t>
         </is>
@@ -493,19 +498,22 @@
         </is>
       </c>
       <c r="E2" t="n">
+        <v>6</v>
+      </c>
+      <c r="F2" t="n">
         <v>1</v>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
+        <is>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
         <is>
           <t>Apply knowledge of core debates surrounding globalisation to analyse contemporary case studies.</t>
         </is>
@@ -529,21 +537,24 @@
         </is>
       </c>
       <c r="E3" t="n">
+        <v>6</v>
+      </c>
+      <c r="F3" t="n">
         <v>2</v>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Apply theories of globalisation to explain observed changes in labour markets and workplace restructuring.</t>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Demonstrate how globalisation impacts labour market and workplace restructuring through the analysis of specific industry examples.</t>
         </is>
       </c>
     </row>
@@ -565,12 +576,10 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>NEEDS_REVISION</t>
-        </is>
+        <v>6</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -579,7 +588,12 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Utilise knowledge of key organisations and institutions involved in globalisation to assess their impact on specific work contexts.</t>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Utilise knowledge of key organisations and institutions involved in globalisation to assess their impact on specific work practices.</t>
         </is>
       </c>
     </row>
@@ -601,19 +615,22 @@
         </is>
       </c>
       <c r="E5" t="n">
+        <v>6</v>
+      </c>
+      <c r="F5" t="n">
         <v>4</v>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>NEEDS_REVISION</t>
-        </is>
-      </c>
       <c r="G5" t="inlineStr">
         <is>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
           <t>COULD_IMPROVE</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>Compare and contrast the impact of globalisation on worker identity in different national contexts.</t>
         </is>
@@ -637,19 +654,22 @@
         </is>
       </c>
       <c r="E6" t="n">
+        <v>6</v>
+      </c>
+      <c r="F6" t="n">
         <v>5</v>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
+        <is>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
         <is>
           <t>Construct arguments evaluating the effectiveness of individual and collective responses to the challenges posed by globalisation in the workplace.</t>
         </is>
@@ -675,10 +695,8 @@
       <c r="E7" t="n">
         <v>6</v>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
+      <c r="F7" t="n">
+        <v>6</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -686,6 +704,11 @@
         </is>
       </c>
       <c r="H7" t="inlineStr">
+        <is>
+          <t>GOOD</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
         <is>
           <t>demonstrate enhanced written, oral and information literacy skills through participation in class discussions, and through the preparation of an individual essay and written responses in the final examination</t>
         </is>
@@ -709,21 +732,24 @@
         </is>
       </c>
       <c r="E8" t="n">
+        <v>6</v>
+      </c>
+      <c r="F8" t="n">
         <v>1</v>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Define key psychological processes and identify their associated measurement techniques.</t>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Define key psychological processes and identify their relationship to brain function.</t>
         </is>
       </c>
     </row>
@@ -745,19 +771,22 @@
         </is>
       </c>
       <c r="E9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F9" t="n">
         <v>2</v>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G9" t="inlineStr">
         <is>
           <t>GOOD</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
+        <is>
+          <t>GOOD</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
         <is>
           <t>identify the basic principles of psychological measurement and experimental design</t>
         </is>
@@ -781,19 +810,22 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
+        <v>6</v>
+      </c>
+      <c r="F10" t="n">
+        <v>3</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
+        <is>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
         <is>
           <t>List types of data used in psychological research and state their basic characteristics.</t>
         </is>
@@ -817,13 +849,11 @@
         </is>
       </c>
       <c r="E11" t="n">
+        <v>6</v>
+      </c>
+      <c r="F11" t="n">
         <v>4</v>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>NEEDS_REVISION</t>
-        </is>
-      </c>
       <c r="G11" t="inlineStr">
         <is>
           <t>NEEDS_REVISION</t>
@@ -831,7 +861,12 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Name the key sections of a research report in APA style.</t>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>List the key components of a research report in APA style.</t>
         </is>
       </c>
     </row>
@@ -853,21 +888,24 @@
         </is>
       </c>
       <c r="E12" t="n">
+        <v>6</v>
+      </c>
+      <c r="F12" t="n">
         <v>5</v>
       </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>NEEDS_REVISION</t>
-        </is>
-      </c>
       <c r="G12" t="inlineStr">
         <is>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
           <t>COULD_IMPROVE</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>Define core psychological terminology.</t>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Define key terms used in psychological science.</t>
         </is>
       </c>
     </row>
@@ -889,19 +927,22 @@
         </is>
       </c>
       <c r="E13" t="n">
+        <v>6</v>
+      </c>
+      <c r="F13" t="n">
         <v>1</v>
       </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>NEEDS_REVISION</t>
-        </is>
-      </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>GOOD</t>
+          <t>NEEDS_REVISION</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
+        <is>
+          <t>GOOD</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
         <is>
           <t>identify and explain the roles and components of AIS</t>
         </is>
@@ -925,21 +966,24 @@
         </is>
       </c>
       <c r="E14" t="n">
+        <v>6</v>
+      </c>
+      <c r="F14" t="n">
         <v>2</v>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>COULD_IMPROVE</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>COULD_IMPROVE</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>describe the role of an internal control system in maintaining data integrity and *explain* potential improvements to protect key business processes.</t>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>describe the role of an internal control system in maintaining data integrity and explain how improvements could protect key business processes.</t>
         </is>
       </c>
     </row>
@@ -961,21 +1005,24 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
+        <v>6</v>
+      </c>
+      <c r="F15" t="n">
+        <v>3</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>compare and contrast business processes and system documentation, identifying key strengths and weaknesses.</t>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>compare and contrast different business processes and system documentation.</t>
         </is>
       </c>
     </row>
@@ -997,21 +1044,24 @@
         </is>
       </c>
       <c r="E16" t="n">
+        <v>6</v>
+      </c>
+      <c r="F16" t="n">
         <v>4</v>
       </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>explain basic data analytics and visualisation techniques and their potential to enhance communication.</t>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>explain basic data analytics and visualisation techniques and their impact on communication.</t>
         </is>
       </c>
     </row>
@@ -1033,19 +1083,22 @@
         </is>
       </c>
       <c r="E17" t="n">
+        <v>6</v>
+      </c>
+      <c r="F17" t="n">
         <v>5</v>
       </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G17" t="inlineStr">
         <is>
           <t>GOOD</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
+        <is>
+          <t>GOOD</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
         <is>
           <t>explain the impact of ICT on current and emerging accounting practices</t>
         </is>
@@ -1071,10 +1124,8 @@
       <c r="E18" t="n">
         <v>6</v>
       </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>NEEDS_REVISION</t>
-        </is>
+      <c r="F18" t="n">
+        <v>6</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1083,7 +1134,12 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>describe the key skills required to work effectively in teams to resolve ICT issues.</t>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>describe the key skills needed to work effectively in teams to resolve ICT issues.</t>
         </is>
       </c>
     </row>
@@ -1105,19 +1161,22 @@
         </is>
       </c>
       <c r="E19" t="n">
+        <v>6</v>
+      </c>
+      <c r="F19" t="n">
         <v>1</v>
       </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>NEEDS_REVISION</t>
-        </is>
-      </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>GOOD</t>
+          <t>NEEDS_REVISION</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
+        <is>
+          <t>GOOD</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
         <is>
           <t>explain the origins of the SDGs and their role in achieving global UN goals;</t>
         </is>
@@ -1141,13 +1200,11 @@
         </is>
       </c>
       <c r="E20" t="n">
+        <v>6</v>
+      </c>
+      <c r="F20" t="n">
         <v>2</v>
       </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>NEEDS_REVISION</t>
-        </is>
-      </c>
       <c r="G20" t="inlineStr">
         <is>
           <t>NEEDS_REVISION</t>
@@ -1155,7 +1212,12 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Relate knowledge of the 17 SDGs to examples of international law and policy.</t>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Compare and contrast the 17 SDGs, describing their relationship with international law and policy.</t>
         </is>
       </c>
     </row>
@@ -1177,21 +1239,24 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
+        <v>6</v>
+      </c>
+      <c r="F21" t="n">
+        <v>3</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Apply understanding of the SDGs to analyse case studies of global and national initiatives.</t>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Apply understanding of the SDGs to evaluate their potential significance and effectiveness at the global and national level.</t>
         </is>
       </c>
     </row>
@@ -1213,21 +1278,24 @@
         </is>
       </c>
       <c r="E22" t="n">
+        <v>6</v>
+      </c>
+      <c r="F22" t="n">
         <v>4</v>
       </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G22" t="inlineStr">
         <is>
+          <t>GOOD</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
           <t>COULD_IMPROVE</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>Demonstrate the application of legal terminology and research findings in written and oral presentations related to the SDGs.</t>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Demonstrate effective oral and written communication skills through the preparation of legal reports and presentations.</t>
         </is>
       </c>
     </row>
@@ -1249,19 +1317,22 @@
         </is>
       </c>
       <c r="E23" t="n">
+        <v>6</v>
+      </c>
+      <c r="F23" t="n">
         <v>5</v>
       </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G23" t="inlineStr">
         <is>
           <t>GOOD</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
+        <is>
+          <t>GOOD</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
         <is>
           <t>develop and apply skills in independent scholarly research</t>
         </is>
@@ -1285,19 +1356,22 @@
         </is>
       </c>
       <c r="E24" t="n">
+        <v>6</v>
+      </c>
+      <c r="F24" t="n">
         <v>1</v>
       </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>NEEDS_REVISION</t>
-        </is>
-      </c>
       <c r="G24" t="inlineStr">
         <is>
           <t>NEEDS_REVISION</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
+        <is>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
         <is>
           <t>Explain the core principles of information literacy and demonstrate their application in evaluating sources.</t>
         </is>
@@ -1321,19 +1395,22 @@
         </is>
       </c>
       <c r="E25" t="n">
+        <v>6</v>
+      </c>
+      <c r="F25" t="n">
         <v>2</v>
       </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>NEEDS_REVISION</t>
-        </is>
-      </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>GOOD</t>
+          <t>NEEDS_REVISION</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
+        <is>
+          <t>GOOD</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
         <is>
           <t>demonstrate a familiarity with basic set theory, relations, functions, predicate logic, correctness proofs, finite state automata and automata theory as tools used in computer science and software engineering</t>
         </is>
@@ -1357,12 +1434,10 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>NEEDS_REVISION</t>
-        </is>
+        <v>6</v>
+      </c>
+      <c r="F26" t="n">
+        <v>3</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1370,6 +1445,11 @@
         </is>
       </c>
       <c r="H26" t="inlineStr">
+        <is>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
         <is>
           <t>Describe how mathematical models can be used to represent problems in computer science and software engineering.</t>
         </is>
@@ -1393,21 +1473,24 @@
         </is>
       </c>
       <c r="E27" t="n">
+        <v>6</v>
+      </c>
+      <c r="F27" t="n">
         <v>4</v>
       </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G27" t="inlineStr">
         <is>
+          <t>GOOD</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
           <t>COULD_IMPROVE</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>Explain how logical reasoning can be applied to solve problems in software engineering.</t>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Explain how logical reasoning can be applied to solve specific problems in software engineering.</t>
         </is>
       </c>
     </row>
@@ -1429,19 +1512,22 @@
         </is>
       </c>
       <c r="E28" t="n">
+        <v>6</v>
+      </c>
+      <c r="F28" t="n">
         <v>1</v>
       </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
+        <is>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
         <is>
           <t>Identify key arguments presented in philosophical texts.</t>
         </is>
@@ -1465,19 +1551,22 @@
         </is>
       </c>
       <c r="E29" t="n">
+        <v>6</v>
+      </c>
+      <c r="F29" t="n">
         <v>2</v>
       </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
+        <is>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
         <is>
           <t>List the core components of a philosophical argument.</t>
         </is>
@@ -1501,19 +1590,22 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
+        <v>6</v>
+      </c>
+      <c r="F30" t="n">
+        <v>3</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
+        <is>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
         <is>
           <t>Define the methodologies used in contemporary philosophy.</t>
         </is>
@@ -1537,19 +1629,22 @@
         </is>
       </c>
       <c r="E31" t="n">
+        <v>6</v>
+      </c>
+      <c r="F31" t="n">
         <v>4</v>
       </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
+        <is>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
         <is>
           <t>State the basic assumptions of common ethical theories.</t>
         </is>
@@ -1573,19 +1668,22 @@
         </is>
       </c>
       <c r="E32" t="n">
+        <v>6</v>
+      </c>
+      <c r="F32" t="n">
         <v>5</v>
       </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
+        <is>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
         <is>
           <t>Recall the steps involved in conducting basic philosophical research.</t>
         </is>
@@ -1611,17 +1709,20 @@
       <c r="E33" t="n">
         <v>6</v>
       </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>NEEDS_REVISION</t>
-        </is>
+      <c r="F33" t="n">
+        <v>6</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
           <t>COULD_IMPROVE</t>
         </is>
       </c>
-      <c r="H33" t="inlineStr">
+      <c r="I33" t="inlineStr">
         <is>
           <t>List important historical and contemporary philosophical ideas in moral philosophy.</t>
         </is>
@@ -1645,19 +1746,22 @@
         </is>
       </c>
       <c r="E34" t="n">
+        <v>6</v>
+      </c>
+      <c r="F34" t="n">
         <v>7</v>
       </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>NEEDS_REVISION</t>
-        </is>
-      </c>
       <c r="G34" t="inlineStr">
         <is>
           <t>NEEDS_REVISION</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
+        <is>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
         <is>
           <t>Name contemporary ethical problems related to digital technologies.</t>
         </is>
@@ -1681,13 +1785,11 @@
         </is>
       </c>
       <c r="E35" t="n">
+        <v>6</v>
+      </c>
+      <c r="F35" t="n">
         <v>8</v>
       </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>NEEDS_REVISION</t>
-        </is>
-      </c>
       <c r="G35" t="inlineStr">
         <is>
           <t>NEEDS_REVISION</t>
@@ -1695,7 +1797,12 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Define several influential ethical theories.</t>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Identify several influential ethical theories.</t>
         </is>
       </c>
     </row>
@@ -1717,21 +1824,24 @@
         </is>
       </c>
       <c r="E36" t="n">
+        <v>6</v>
+      </c>
+      <c r="F36" t="n">
         <v>9</v>
       </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Identify which ethical theories are relevant to problems in digital technologies.</t>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>Describe how ethical theories can be used to address problems in digital technologies.</t>
         </is>
       </c>
     </row>
@@ -1753,21 +1863,24 @@
         </is>
       </c>
       <c r="E37" t="n">
+        <v>6</v>
+      </c>
+      <c r="F37" t="n">
         <v>10</v>
       </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>List the steps involved in applying ethical theories to new questions.</t>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>Define key terms related to ethical reasoning.</t>
         </is>
       </c>
     </row>
@@ -1789,19 +1902,22 @@
         </is>
       </c>
       <c r="E38" t="n">
+        <v>6</v>
+      </c>
+      <c r="F38" t="n">
         <v>1</v>
       </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>NEEDS_REVISION</t>
-        </is>
-      </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>GOOD</t>
+          <t>NEEDS_REVISION</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
+        <is>
+          <t>GOOD</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
         <is>
           <t>demonstrate professional engineering skills and abilities when working in teams</t>
         </is>
@@ -1825,21 +1941,24 @@
         </is>
       </c>
       <c r="E39" t="n">
+        <v>6</v>
+      </c>
+      <c r="F39" t="n">
         <v>2</v>
       </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>NEEDS_REVISION</t>
-        </is>
-      </c>
       <c r="G39" t="inlineStr">
         <is>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
           <t>COULD_IMPROVE</t>
         </is>
       </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>Develop and validate models of power systems components (transmission lines, transformers, generators and loads) for system analysis.</t>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Develop and validate models of power systems components (transmission lines, transformers, generators and loads) for use in system analysis.</t>
         </is>
       </c>
     </row>
@@ -1861,12 +1980,10 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>NEEDS_REVISION</t>
-        </is>
+        <v>6</v>
+      </c>
+      <c r="F40" t="n">
+        <v>3</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -1874,6 +1991,11 @@
         </is>
       </c>
       <c r="H40" t="inlineStr">
+        <is>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
         <is>
           <t>Design a power flow analysis strategy for a simple interconnected power system, justifying the selection of Gauss-Siedal, Newton Raphson, or decoupled power flow methods based on system characteristics.</t>
         </is>
@@ -1897,19 +2019,22 @@
         </is>
       </c>
       <c r="E41" t="n">
+        <v>6</v>
+      </c>
+      <c r="F41" t="n">
         <v>4</v>
       </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
+        <is>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
         <is>
           <t>Propose and justify modifications to a power network design to mitigate the impact of short-circuit faults, considering various fault current control strategies.</t>
         </is>
@@ -1933,21 +2058,24 @@
         </is>
       </c>
       <c r="E42" t="n">
+        <v>6</v>
+      </c>
+      <c r="F42" t="n">
         <v>5</v>
       </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Develop a comprehensive protection scheme for a power transmission and distribution system, integrating multiple protection techniques to address various fault scenarios.</t>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>Develop a comprehensive protection scheme for a power transmission and distribution system, integrating multiple protection techniques and justifying their selection.</t>
         </is>
       </c>
     </row>
@@ -1971,19 +2099,22 @@
       <c r="E43" t="n">
         <v>6</v>
       </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
+      <c r="F43" t="n">
+        <v>6</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Formulate a control strategy for maintaining voltage and frequency stability in an interconnected power system, combining different control techniques and anticipating potential disturbances.</t>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>Formulate a control strategy for maintaining voltage and frequency stability in an interconnected power system, considering dynamic system responses.</t>
         </is>
       </c>
     </row>
@@ -2005,21 +2136,24 @@
         </is>
       </c>
       <c r="E44" t="n">
+        <v>6</v>
+      </c>
+      <c r="F44" t="n">
         <v>7</v>
       </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Develop a comprehensive safety plan for a power systems laboratory or field work, integrating hazard identification, risk assessment, and appropriate mitigation measures.</t>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>Develop a comprehensive safety plan for working with power systems equipment, integrating hazard identification, risk assessment, and mitigation strategies.</t>
         </is>
       </c>
     </row>
@@ -2041,19 +2175,22 @@
         </is>
       </c>
       <c r="E45" t="n">
+        <v>6</v>
+      </c>
+      <c r="F45" t="n">
         <v>1</v>
       </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
+        <is>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
         <is>
           <t>Describe the concepts and physical principles related to magnetism, the foundations of quantum mechanics and electronic properties of materials.</t>
         </is>
@@ -2077,19 +2214,22 @@
         </is>
       </c>
       <c r="E46" t="n">
+        <v>6</v>
+      </c>
+      <c r="F46" t="n">
         <v>2</v>
       </c>
-      <c r="F46" t="inlineStr">
+      <c r="G46" t="inlineStr">
         <is>
           <t>COULD_IMPROVE</t>
         </is>
       </c>
-      <c r="G46" t="inlineStr">
+      <c r="H46" t="inlineStr">
         <is>
           <t>COULD_IMPROVE</t>
         </is>
       </c>
-      <c r="H46" t="inlineStr">
+      <c r="I46" t="inlineStr">
         <is>
           <t>Explain, in both oral and written form, the key concepts related to magnetism, the foundations of quantum mechanics and electronic devices.</t>
         </is>
@@ -2113,21 +2253,24 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
+        <v>6</v>
+      </c>
+      <c r="F47" t="n">
+        <v>3</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Illustrate how the principles of magnetism, quantum mechanics, and electronic properties of materials apply to simple scenarios.</t>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>Illustrate how the principles of magnetism, quantum mechanics and electronic properties of materials apply to simple scenarios.</t>
         </is>
       </c>
     </row>
@@ -2149,21 +2292,24 @@
         </is>
       </c>
       <c r="E48" t="n">
+        <v>6</v>
+      </c>
+      <c r="F48" t="n">
         <v>4</v>
       </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>COULD_IMPROVE</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Describe the procedures for conducting experiments relevant to magnetism and electronic devices.</t>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>Describe the procedures for experiments relevant to magnetism and electronic devices.</t>
         </is>
       </c>
     </row>
@@ -2185,13 +2331,11 @@
         </is>
       </c>
       <c r="E49" t="n">
+        <v>6</v>
+      </c>
+      <c r="F49" t="n">
         <v>5</v>
       </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>NEEDS_REVISION</t>
-        </is>
-      </c>
       <c r="G49" t="inlineStr">
         <is>
           <t>NEEDS_REVISION</t>
@@ -2199,7 +2343,12 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Summarise the results of an experiment related to magnetism and electronic devices.</t>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Summarise the results of an experiment relating to magnetism and electronic devices.</t>
         </is>
       </c>
     </row>
@@ -2221,19 +2370,22 @@
         </is>
       </c>
       <c r="E50" t="n">
+        <v>6</v>
+      </c>
+      <c r="F50" t="n">
         <v>1</v>
       </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G50" t="inlineStr">
         <is>
+          <t>GOOD</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
           <t>COULD_IMPROVE</t>
         </is>
       </c>
-      <c r="H50" t="inlineStr">
+      <c r="I50" t="inlineStr">
         <is>
           <t>Apply knowledge of clinical signs, symptoms and pathogenesis of systemic conditions to develop appropriate dental treatment plans.</t>
         </is>
@@ -2257,19 +2409,22 @@
         </is>
       </c>
       <c r="E51" t="n">
+        <v>6</v>
+      </c>
+      <c r="F51" t="n">
         <v>2</v>
       </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
+        <is>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
         <is>
           <t>Utilise understanding of microbial pathogenicity and transmission to implement infection control protocols in a dental setting.</t>
         </is>
@@ -2293,12 +2448,10 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>3</v>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
+        <v>6</v>
+      </c>
+      <c r="F52" t="n">
+        <v>3</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2306,6 +2459,11 @@
         </is>
       </c>
       <c r="H52" t="inlineStr">
+        <is>
+          <t>GOOD</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
         <is>
           <t>apply the principles of infection prevention and control in dental practice, including when treating patients with communicable diseases</t>
         </is>
@@ -2329,19 +2487,22 @@
         </is>
       </c>
       <c r="E53" t="n">
+        <v>6</v>
+      </c>
+      <c r="F53" t="n">
         <v>4</v>
       </c>
-      <c r="F53" t="inlineStr">
+      <c r="G53" t="inlineStr">
         <is>
           <t>COULD_IMPROVE</t>
         </is>
       </c>
-      <c r="G53" t="inlineStr">
+      <c r="H53" t="inlineStr">
         <is>
           <t>COULD_IMPROVE</t>
         </is>
       </c>
-      <c r="H53" t="inlineStr">
+      <c r="I53" t="inlineStr">
         <is>
           <t>Implement appropriate modifications to dental treatment plans based on patient</t>
         </is>
@@ -2365,21 +2526,24 @@
         </is>
       </c>
       <c r="E54" t="n">
+        <v>6</v>
+      </c>
+      <c r="F54" t="n">
         <v>5</v>
       </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>COULD_IMPROVE</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Apply classification of medical emergencies to effectively manage simulated emergency scenarios in a dental practice.</t>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>Demonstrate the correct procedures for managing common medical emergencies encountered in a dental practice.</t>
         </is>
       </c>
     </row>
@@ -2403,19 +2567,22 @@
       <c r="E55" t="n">
         <v>6</v>
       </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
+      <c r="F55" t="n">
+        <v>6</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Calculate appropriate drug dosages and delivery methods for common dental procedures, considering patient-specific factors.</t>
+          <t>COULD_IMPROVE</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>Select appropriate medications and dosages for dental procedures, considering drug delivery and metabolism.</t>
         </is>
       </c>
     </row>
@@ -2437,19 +2604,22 @@
         </is>
       </c>
       <c r="E56" t="n">
+        <v>6</v>
+      </c>
+      <c r="F56" t="n">
         <v>7</v>
       </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G56" t="inlineStr">
         <is>
+          <t>GOOD</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
           <t>COULD_IMPROVE</t>
         </is>
       </c>
-      <c r="H56" t="inlineStr">
+      <c r="I56" t="inlineStr">
         <is>
           <t>Modify dental treatment plans to account for potential drug interactions and patient medication profiles.</t>
         </is>
@@ -2473,21 +2643,24 @@
         </is>
       </c>
       <c r="E57" t="n">
+        <v>6</v>
+      </c>
+      <c r="F57" t="n">
         <v>8</v>
       </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Select appropriate medications for pain management or infection control in dental treatment, justifying choices based on indications and contraindications.</t>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>Utilise knowledge of common dental medications to safely and effectively manage patient prescriptions and potential adverse reactions.</t>
         </is>
       </c>
     </row>
@@ -2509,21 +2682,24 @@
         </is>
       </c>
       <c r="E58" t="n">
+        <v>6</v>
+      </c>
+      <c r="F58" t="n">
         <v>9</v>
       </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G58" t="inlineStr">
         <is>
+          <t>GOOD</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
           <t>COULD_IMPROVE</t>
         </is>
       </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>Complete a prescription accurately and legally, adhering to relevant regulatory requirements.</t>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>Complete and accurately write prescriptions adhering to all relevant regulatory requirements.</t>
         </is>
       </c>
     </row>
@@ -2545,21 +2721,24 @@
         </is>
       </c>
       <c r="E59" t="n">
+        <v>6</v>
+      </c>
+      <c r="F59" t="n">
         <v>10</v>
       </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Demonstrate effective communication and ethical decision-making in simulated clinical scenarios.</t>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>Demonstrate effective communication and ethical decision-making in simulated dental patient interactions.</t>
         </is>
       </c>
     </row>
@@ -2581,19 +2760,22 @@
         </is>
       </c>
       <c r="E60" t="n">
+        <v>6</v>
+      </c>
+      <c r="F60" t="n">
         <v>1</v>
       </c>
-      <c r="F60" t="inlineStr">
+      <c r="G60" t="inlineStr">
         <is>
           <t>COULD_IMPROVE</t>
         </is>
       </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="H60" t="inlineStr">
+        <is>
+          <t>GOOD</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
         <is>
           <t>demonstrate an ability to work effectively in laboratory teams</t>
         </is>
@@ -2617,19 +2799,22 @@
         </is>
       </c>
       <c r="E61" t="n">
+        <v>6</v>
+      </c>
+      <c r="F61" t="n">
         <v>2</v>
       </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
+        <is>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
         <is>
           <t>Apply the principles of EMF generation and torque to explain the operation of motors and generators.</t>
         </is>
@@ -2653,19 +2838,22 @@
         </is>
       </c>
       <c r="E62" t="n">
-        <v>3</v>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
+        <v>6</v>
+      </c>
+      <c r="F62" t="n">
+        <v>3</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
+        <is>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
         <is>
           <t>Calculate the performance characteristics (regulation, losses, and efficiency) of DC machines, transformers, induction, and synchronous machines using equivalent circuit parameters.</t>
         </is>
@@ -2689,19 +2877,22 @@
         </is>
       </c>
       <c r="E63" t="n">
+        <v>6</v>
+      </c>
+      <c r="F63" t="n">
         <v>4</v>
       </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>NEEDS_REVISION</t>
-        </is>
-      </c>
       <c r="G63" t="inlineStr">
         <is>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
           <t>COULD_IMPROVE</t>
         </is>
       </c>
-      <c r="H63" t="inlineStr">
+      <c r="I63" t="inlineStr">
         <is>
           <t>Use phasor diagrams to illustrate the working principles of transformers and AC electrical machines.</t>
         </is>
@@ -2725,19 +2916,22 @@
         </is>
       </c>
       <c r="E64" t="n">
+        <v>6</v>
+      </c>
+      <c r="F64" t="n">
         <v>5</v>
       </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
+        <is>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
         <is>
           <t>Apply torque-speed characteristics to select appropriate speed control techniques for DC and induction motors.</t>
         </is>
@@ -2763,17 +2957,20 @@
       <c r="E65" t="n">
         <v>6</v>
       </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
+      <c r="F65" t="n">
+        <v>6</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>NEEDS_REVISION</t>
+          <t>GOOD</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
+        <is>
+          <t>NEEDS_REVISION</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
         <is>
           <t>Calculate transmission line parameters and represent power systems using appropriate models.</t>
         </is>
@@ -2797,19 +2994,22 @@
         </is>
       </c>
       <c r="E66" t="n">
+        <v>6</v>
+      </c>
+      <c r="F66" t="n">
         <v>7</v>
       </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>GOOD</t>
-        </is>
-      </c>
       <c r="G66" t="inlineStr">
         <is>
           <t>GOOD</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
+        <is>
+          <t>GOOD</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
         <is>
           <t>demonstrate compliance with work, health and safety regulations, codes and standards when operating electrical machines</t>
         </is>

</xml_diff>